<commit_message>
2014 03 16   00:31
</commit_message>
<xml_diff>
--- a/BD2_2M/T1 - View/Agenda de projeto.xlsx
+++ b/BD2_2M/T1 - View/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15975" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$J$22</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -161,8 +161,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -417,17 +417,17 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,7 +435,60 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1047" name="Rectangle 23" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,6 +566,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -547,6 +601,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -722,18 +777,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="22" customWidth="1"/>
     <col min="2" max="2" width="57" style="22" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="25" customWidth="1"/>
     <col min="4" max="4" width="12" style="21" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="21" customWidth="1"/>
     <col min="6" max="7" width="12.7109375" style="21" customWidth="1"/>
@@ -744,22 +799,22 @@
     <col min="12" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="20" customFormat="1" ht="15">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:11" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="7"/>
       <c r="J1" s="8"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="14.25">
+    <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11"/>
@@ -772,7 +827,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:11" ht="33.75" customHeight="1">
+    <row r="3" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -807,7 +862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="24" customHeight="1">
+    <row r="4" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -834,7 +889,7 @@
       </c>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="24" customHeight="1">
+    <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -861,7 +916,7 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="24" customHeight="1">
+    <row r="6" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -881,21 +936,21 @@
         <v>14</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1">
+    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="26" t="str">
+      <c r="C7" s="24" t="str">
         <f>B6</f>
         <v>Tabela Aluno</v>
       </c>
@@ -916,7 +971,7 @@
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1">
+    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -943,7 +998,7 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1">
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -971,7 +1026,7 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1">
+    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -998,7 +1053,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="24" customHeight="1">
+    <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1026,7 +1081,7 @@
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="24" customHeight="1">
+    <row r="12" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1049,7 +1104,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="24" customHeight="1">
+    <row r="13" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1131,7 @@
       </c>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="24" customHeight="1">
+    <row r="14" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1103,7 +1158,7 @@
       </c>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" ht="24" customHeight="1">
+    <row r="15" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1130,7 +1185,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="24" customHeight="1">
+    <row r="16" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1157,7 +1212,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="24" customHeight="1">
+    <row r="17" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1184,7 +1239,7 @@
       </c>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" ht="24" customHeight="1">
+    <row r="18" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
@@ -1197,7 +1252,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" ht="26.25" customHeight="1">
+    <row r="19" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
@@ -1210,7 +1265,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" ht="26.25" customHeight="1">
+    <row r="20" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
@@ -1223,7 +1278,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="26.25" customHeight="1">
+    <row r="21" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
@@ -1236,7 +1291,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="26.25" customHeight="1">
+    <row r="22" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
@@ -1249,7 +1304,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" s="23" customFormat="1" ht="26.25" customHeight="1">
+    <row r="23" spans="1:11" s="23" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
@@ -1269,6 +1324,7 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2014 03 16   03:41
</commit_message>
<xml_diff>
--- a/BD2_2M/T1 - View/Agenda de projeto.xlsx
+++ b/BD2_2M/T1 - View/Agenda de projeto.xlsx
@@ -149,13 +149,13 @@
     <t>Insert de 10 aunos</t>
   </si>
   <si>
-    <t xml:space="preserve">Insert de 5 disciplinas </t>
-  </si>
-  <si>
     <t>Insert de 10 matriculas</t>
   </si>
   <si>
     <t>Atividades estão detalhadas no arquivo "02 Exercício de View em PostgreSQL ALUNO x DISCIPLINA.pdf"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserir 5 disciplinas </t>
   </si>
 </sst>
 </file>
@@ -202,7 +202,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +332,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -427,6 +433,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -461,6 +470,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="1047" name="Rectangle 23" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 23" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -781,7 +833,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -789,9 +841,10 @@
     <col min="1" max="1" width="8.7109375" style="22" customWidth="1"/>
     <col min="2" max="2" width="57" style="22" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="12" style="21" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="21" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="21" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" style="21" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" style="21" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" style="22" customWidth="1"/>
@@ -801,7 +854,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="27"/>
@@ -960,11 +1013,11 @@
       <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="28" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>19</v>
@@ -987,11 +1040,11 @@
       <c r="G8" s="3">
         <v>4</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="28" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>19</v>
@@ -1003,7 +1056,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>B8</f>
@@ -1019,7 +1072,7 @@
         <v>14</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>19</v>
@@ -1058,7 +1111,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>B10</f>

</xml_diff>

<commit_message>
2014 03 17 07:57
</commit_message>
<xml_diff>
--- a/BD2_2M/T1 - View/Agenda de projeto.xlsx
+++ b/BD2_2M/T1 - View/Agenda de projeto.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="600" windowWidth="15975" windowHeight="8640"/>
+    <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$J$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$22</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -22,7 +22,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0">
+    <comment ref="F3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
   <si>
     <t>Ação</t>
   </si>
@@ -53,15 +53,6 @@
     <t>Local criação</t>
   </si>
   <si>
-    <t>Atributo</t>
-  </si>
-  <si>
-    <t>Tipo atributo</t>
-  </si>
-  <si>
-    <t>Desc atributo</t>
-  </si>
-  <si>
     <t>Fase de execução</t>
   </si>
   <si>
@@ -156,13 +147,19 @@
   </si>
   <si>
     <t xml:space="preserve">Inserir 5 disciplinas </t>
+  </si>
+  <si>
+    <t>Os ids de disciplina e aluno são ficticios</t>
+  </si>
+  <si>
+    <t>Ativid:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -354,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -429,14 +426,17 @@
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,7 +462,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
@@ -505,7 +505,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
@@ -618,7 +618,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -653,7 +652,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -829,58 +827,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="22" customWidth="1"/>
     <col min="2" max="2" width="57" style="22" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="25" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="21" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="21" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="21" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="22" customWidth="1"/>
-    <col min="11" max="11" width="46.5703125" style="22" customWidth="1"/>
-    <col min="12" max="16384" width="9.85546875" style="2"/>
+    <col min="4" max="4" width="15.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="21" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="46.5703125" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="20" customFormat="1" ht="15">
+      <c r="A1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="33.75" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -902,478 +891,418 @@
       <c r="G3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="15" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="24" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="F4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="24" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="24" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="F6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="24" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="24" t="str">
         <f>B6</f>
         <v>Tabela Aluno</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="24" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3">
         <v>4</v>
       </c>
-      <c r="H8" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="24" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>B8</f>
         <v>Tabela Disciplina</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3">
+      <c r="D9" s="3">
         <v>4</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="24" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="24" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>B10</f>
         <v>Tabela AluDis</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3">
+      <c r="D11" s="3">
         <v>5</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="24" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="F13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="24" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="24" customHeight="1">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="3">
-        <v>6</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3">
-        <v>7</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="F15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="24" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="F16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3">
-        <v>8</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="24" customHeight="1">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3">
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3">
-        <v>10</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3">
-        <v>11</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="24" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="26.25" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="26.25" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="26.25" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="26.25" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" s="23" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" s="23" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A23" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="29">
+        <f>COUNTA(B4:B22)</f>
+        <v>14</v>
+      </c>
       <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:J22"/>
+  <autoFilter ref="A3:G22"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
2014 03 16 18:22
Criação da tabela avaliçãoes
</commit_message>
<xml_diff>
--- a/BD2_2M/T1 - View/Agenda de projeto.xlsx
+++ b/BD2_2M/T1 - View/Agenda de projeto.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$24</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="39">
   <si>
     <t>Ação</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Ativid:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabela avaliação </t>
+  </si>
+  <si>
+    <t>Nescessaria para calcular a média do da view conceito</t>
   </si>
 </sst>
 </file>
@@ -429,14 +435,14 @@
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +470,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -507,7 +513,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -828,10 +834,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -843,18 +850,18 @@
     <col min="5" max="5" width="17.7109375" style="21" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="21" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="46.5703125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="53" style="22" customWidth="1"/>
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="20" customFormat="1" ht="15">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
       <c r="F1" s="7"/>
       <c r="G1" s="8"/>
       <c r="H1" s="7"/>
@@ -895,7 +902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24" customHeight="1">
+    <row r="4" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -919,7 +926,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="24" customHeight="1">
+    <row r="5" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -943,7 +950,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="24" customHeight="1">
+    <row r="6" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -967,7 +974,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="24" customHeight="1">
+    <row r="7" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -992,7 +999,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="24" customHeight="1">
+    <row r="8" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1016,7 +1023,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="24" customHeight="1">
+    <row r="9" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1041,7 +1048,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="24" customHeight="1">
+    <row r="10" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1064,7 +1071,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="24" customHeight="1">
+    <row r="11" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1114,7 +1121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="24" customHeight="1">
+    <row r="13" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1162,42 +1169,44 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="24" customHeight="1">
+    <row r="15" spans="1:8" ht="25.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="3">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="24" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>11</v>
@@ -1210,41 +1219,55 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="24" customHeight="1">
+    <row r="17" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="3">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="24" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="24" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="26.25" customHeight="1">
+    <row r="19" spans="1:8" ht="24" hidden="1" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
@@ -1254,7 +1277,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="26.25" customHeight="1">
+    <row r="20" spans="1:8" ht="26.25" hidden="1" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
@@ -1264,7 +1287,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="26.25" customHeight="1">
+    <row r="21" spans="1:8" ht="26.25" hidden="1" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
@@ -1274,7 +1297,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="26.25" customHeight="1">
+    <row r="22" spans="1:8" ht="26.25" hidden="1" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
@@ -1284,23 +1307,44 @@
       <c r="G22" s="3"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" s="23" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:8" ht="26.25" hidden="1" customHeight="1">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" s="23" customFormat="1" ht="26.25" hidden="1" customHeight="1">
+      <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="29">
-        <f>COUNTA(B4:B22)</f>
-        <v>14</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
+      <c r="B24" s="27">
+        <f>COUNTA(B4:B23)</f>
+        <v>15</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G22"/>
+  <autoFilter ref="A3:G24">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Neimar"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="?"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>

</xml_diff>

<commit_message>
2014 03 16 19:00
Conclusao das view
</commit_message>
<xml_diff>
--- a/BD2_2M/T1 - View/Agenda de projeto.xlsx
+++ b/BD2_2M/T1 - View/Agenda de projeto.xlsx
@@ -834,11 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -902,7 +901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="4" spans="1:8" ht="24" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -926,7 +925,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="5" spans="1:8" ht="24" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -950,7 +949,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="6" spans="1:8" ht="24" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -974,7 +973,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="7" spans="1:8" ht="24" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -999,7 +998,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="8" spans="1:8" ht="24" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1022,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="9" spans="1:8" ht="24" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1048,7 +1047,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="10" spans="1:8" ht="24" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="11" spans="1:8" ht="24" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1115,13 +1114,13 @@
         <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="13" spans="1:8" ht="24" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1162,7 +1161,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>16</v>
@@ -1186,7 +1185,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>16</v>
@@ -1195,7 +1194,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="16" spans="1:8" ht="24" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1219,7 +1218,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="17" spans="1:8" ht="24" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1267,7 +1266,7 @@
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="24" hidden="1" customHeight="1">
+    <row r="19" spans="1:8" ht="24" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
@@ -1277,7 +1276,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="26.25" hidden="1" customHeight="1">
+    <row r="20" spans="1:8" ht="26.25" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
@@ -1287,7 +1286,7 @@
       <c r="G20" s="3"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="26.25" hidden="1" customHeight="1">
+    <row r="21" spans="1:8" ht="26.25" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="3"/>
@@ -1297,7 +1296,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="26.25" hidden="1" customHeight="1">
+    <row r="22" spans="1:8" ht="26.25" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="3"/>
@@ -1307,7 +1306,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="26.25" hidden="1" customHeight="1">
+    <row r="23" spans="1:8" ht="26.25" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="3"/>
@@ -1317,7 +1316,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" s="23" customFormat="1" ht="26.25" hidden="1" customHeight="1">
+    <row r="24" spans="1:8" s="23" customFormat="1" ht="26.25" customHeight="1">
       <c r="A24" s="16" t="s">
         <v>36</v>
       </c>
@@ -1334,16 +1333,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:G24">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Neimar"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="?"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
   </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
2014 03 20 15:30
criação  de weiw
</commit_message>
<xml_diff>
--- a/BD2_2M/T1 - View/Agenda de projeto.xlsx
+++ b/BD2_2M/T1 - View/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$24</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -837,7 +837,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1137,7 +1137,7 @@
         <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>16</v>
@@ -1211,7 +1211,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>25</v>
@@ -1235,7 +1235,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
2014 03 24 20:52
Edição e criação de tabelas
</commit_message>
<xml_diff>
--- a/BD2_2M/T1 - View/Agenda de projeto.xlsx
+++ b/BD2_2M/T1 - View/Agenda de projeto.xlsx
@@ -30,10 +30,13 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Estatus:
-? = Em aberto
-! = Concluida
-?! = Em execução</t>
+          <t>Estatus da atividade:
+========================
+?  = Em aberto
+!   = Concluida
+?! = Em execução
+!!  = Revisado ok
+*  =  Dúvida (Aguarda solução)</t>
         </r>
       </text>
     </comment>
@@ -837,7 +840,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>

</xml_diff>